<commit_message>
add : delete speech bubble
- 일정 시간이 지나면 생성했던 말풍선 오브젝트 삭제
</commit_message>
<xml_diff>
--- a/Assets/Resources/DataFiles/DialogDataFile.xlsx
+++ b/Assets/Resources/DataFiles/DialogDataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bluejoy\Documents\GitHub\Tycoon\Assets\Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bluejoy\Documents\GitHub\Tycoon\Assets\Resources\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E7CABB3-62D6-40C4-9835-0CB7B3CD1D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660DD104-A445-4FCD-AE91-C955B870407D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{84BA1C68-EE14-4FA3-A308-DE482E31DFFE}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="9970" xr2:uid="{84BA1C68-EE14-4FA3-A308-DE482E31DFFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -736,11 +736,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -759,9 +759,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
@@ -1209,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F83B47-E66A-4F03-98A5-09CCF236256F}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1222,21 +1219,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1244,8 +1241,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="28"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="33" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1253,35 +1250,35 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="29"/>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="28"/>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="33" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1289,36 +1286,36 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="29"/>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="34"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="3"/>
-      <c r="E9" s="15"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="28"/>
-      <c r="B11" s="34" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="33" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1326,466 +1323,466 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="29"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="46"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="29"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="40"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="29"/>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="28"/>
+      <c r="B21" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="43"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="29"/>
-      <c r="B29" s="39" t="s">
+      <c r="A29" s="28"/>
+      <c r="B29" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:5" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="1"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="50"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="49"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="40"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="29"/>
-      <c r="B35" s="39" t="s">
+      <c r="A35" s="28"/>
+      <c r="B35" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="15"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="8"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="29"/>
-      <c r="B38" s="39" t="s">
+      <c r="A38" s="28"/>
+      <c r="B38" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="1"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="50"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="49"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="40"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="8"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="29"/>
-      <c r="B46" s="39" t="s">
+      <c r="A46" s="28"/>
+      <c r="B46" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="9"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="8"/>
     </row>
     <row r="48" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A48" s="1"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="50"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="49"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="45" t="s">
+      <c r="B49" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="40"/>
+      <c r="B50" s="39"/>
       <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" s="29"/>
-      <c r="B52" s="46" t="s">
+      <c r="A52" s="28"/>
+      <c r="B52" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="23" t="s">
+      <c r="C52" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="8"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="7"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="29"/>
-      <c r="B55" s="46" t="s">
+      <c r="A55" s="28"/>
+      <c r="B55" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="37"/>
-      <c r="C56" s="9"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" spans="1:3" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A57" s="1"/>
-      <c r="B57" s="51"/>
-      <c r="C57" s="50"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="49"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="45" t="s">
+      <c r="B58" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="40"/>
+      <c r="B59" s="39"/>
       <c r="C59" s="7"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="38" t="s">
+      <c r="B60" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A61" s="29"/>
-      <c r="B61" s="46" t="s">
+      <c r="A61" s="28"/>
+      <c r="B61" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="8"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="7"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A63" s="30" t="s">
+      <c r="A63" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="38" t="s">
+      <c r="B63" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A64" s="29"/>
-      <c r="B64" s="46" t="s">
+      <c r="A64" s="28"/>
+      <c r="B64" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="37"/>
-      <c r="C65" s="9"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>